<commit_message>
changed the input layer logic to support different support sizes.
</commit_message>
<xml_diff>
--- a/graphCaseUnitTest/check_layer_calc.xlsx
+++ b/graphCaseUnitTest/check_layer_calc.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonpoppe/workspace/GraphCase/graphCaseUnitTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAD8DB7-5A5C-F346-9FA2-309307A9A68E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E645AE-2928-7041-B307-948DCE38DC71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{00042199-49BE-E54D-97D2-5F9F03390C30}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" activeTab="2" xr2:uid="{00042199-49BE-E54D-97D2-5F9F03390C30}"/>
   </bookViews>
   <sheets>
     <sheet name="layer1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="dims" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="40">
   <si>
     <t>i = [10  7  8]</t>
   </si>
@@ -131,6 +132,21 @@
   </si>
   <si>
     <t>[14.69048</t>
+  </si>
+  <si>
+    <t>dim</t>
+  </si>
+  <si>
+    <t>node id of batch</t>
+  </si>
+  <si>
+    <t>hub 1 node ids</t>
+  </si>
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t>hub next node ids</t>
   </si>
 </sst>
 </file>
@@ -489,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0484F16-52EA-1041-B684-0EF1910E00CA}">
   <dimension ref="A1:AH170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J152" workbookViewId="0">
-      <selection activeCell="U165" sqref="U165"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14993,4 +15009,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A984BD9F-CB1F-FC40-A35B-ECB5851CD447}">
+  <dimension ref="C5:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>